<commit_message>
updating robots.txt to add sitemap.xml
</commit_message>
<xml_diff>
--- a/SEO campaign/Rapport-audit-1s.xlsx
+++ b/SEO campaign/Rapport-audit-1s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmation\Web\Openclassroom\project_4\SEO campaign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D2C2F7-D310-448B-9E66-44FC807FD481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD9D2B5-7402-4108-BFC1-8F1C950463FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1200" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="38700" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
   <si>
     <t>Catégorie</t>
   </si>
@@ -665,9 +665,6 @@
   </si>
   <si>
     <t>Formulaire</t>
-  </si>
-  <si>
-    <t>Messages d'erreur en anglais</t>
   </si>
   <si>
     <t>Traduire les messages d'erreur</t>
@@ -808,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -820,14 +817,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1441,53 +1437,74 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>82</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
-        <v>96</v>
+    <row r="20" spans="1:6" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>